<commit_message>
Updates for paper revision 1
</commit_message>
<xml_diff>
--- a/models/Master - Cleanup.xlsx
+++ b/models/Master - Cleanup.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr showInkAnnotation="0" updateLinks="never" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr showInkAnnotation="0" updateLinks="never"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aengholm\MUST code repository\climate_scenarios_EMA\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aengholm\code repos\EMA-transport-climate-policy-SE\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A67D7C-280D-484E-9D8F-ED7E2687DEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18135" yWindow="-16470" windowWidth="29040" windowHeight="15840" tabRatio="752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18135" yWindow="-16470" windowWidth="29040" windowHeight="15840" tabRatio="752" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Beskrivning" sheetId="19" r:id="rId1"/>
@@ -45,7 +44,12 @@
     <definedName name="KALKYLPERIOD" localSheetId="10">'[2]0.12 Lönkalk'!#REF!</definedName>
     <definedName name="KALKYLPERIOD">'[2]0.12 Lönkalk'!#REF!</definedName>
     <definedName name="kr_till_öre">'[1]Koefficienter &amp; omvandlingstal'!$A$20</definedName>
+    <definedName name="M1_CO2_TTW_total">EMA!$C$57</definedName>
+    <definedName name="M2_driving_cost_car">EMA!$C$53</definedName>
+    <definedName name="M3_driving_cost_truck">EMA!$C$54</definedName>
     <definedName name="m3_till_liter">'[1]Koefficienter &amp; omvandlingstal'!$A$21</definedName>
+    <definedName name="M4_energy_use_bio">EMA!$C$41</definedName>
+    <definedName name="M5_energy_use_electricity">EMA!$C$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,35 +72,62 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={EF767CCE-FA5F-48F1-9A64-A0329AA003A2}</author>
     <author>tc={8470CDAA-5119-482B-908E-7232FD2591EE}</author>
     <author>tc={7AA0C079-4270-4107-80A8-167265DE1676}</author>
   </authors>
   <commentList>
-    <comment ref="A64" authorId="0" shapeId="0" xr:uid="{EF767CCE-FA5F-48F1-9A64-A0329AA003A2}">
+    <comment ref="A64" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Exkluderar eventuella intäkter från drivmedelsskatter för bussar </t>
+        </r>
       </text>
     </comment>
-    <comment ref="A73" authorId="1" shapeId="0" xr:uid="{8470CDAA-5119-482B-908E-7232FD2591EE}">
+    <comment ref="A73" authorId="1" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Exkluderar bussar</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A76" authorId="2" shapeId="0" xr:uid="{7AA0C079-4270-4107-80A8-167265DE1676}">
+    <comment ref="A76" authorId="2" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Exkluderar bussar</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -104,7 +135,7 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={AD68DB3D-FDF3-474F-8A95-58C66EF631AE}</author>
     <author>tc={A167A516-C634-44D7-A17A-54F89DEFA376}</author>
@@ -115,60 +146,123 @@
     <author>tc={88AB02D8-4CA1-4C85-B8A3-8EAC71FECC61}</author>
   </authors>
   <commentList>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{AD68DB3D-FDF3-474F-8A95-58C66EF631AE}">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     inkl. etanol och gas</t>
+        </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="1" shapeId="0" xr:uid="{A167A516-C634-44D7-A17A-54F89DEFA376}">
+    <comment ref="F7" authorId="1" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     inkl. etanol och gas</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="2" shapeId="0" xr:uid="{D25970DF-AEBF-4E49-A6DE-2F9749BFC419}">
+    <comment ref="A12" authorId="2" shapeId="0">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Trafikarbetet motsvarar utvecklingstakten i Basprognos 2018 men utifrånTrafikanalys offifiella trafikarbetsstatistik för år 2017. Eftersom befolkningsutvecklingen skrivits upp betydligt sedan BP2018 har även en justering gjorts för att ta höjd för förändringen med +2,5 % år 2030 samt + 5 % år 2040. </t>
+        </r>
       </text>
     </comment>
-    <comment ref="A15" authorId="3" shapeId="0" xr:uid="{8108A131-0058-4CD6-8C5A-35838975E17B}">
+    <comment ref="A15" authorId="3" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Från HBEFA juni 2019 fram till 2030 (och 2035) sedan utvecklingstakt från Scenario Transporteffektivt 20190529</t>
+        </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="4" shapeId="0" xr:uid="{FD325718-70E0-4698-A38F-A47A779DBA26}">
+    <comment ref="F15" authorId="4" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Från HBEFA juni 2019 fram till 2030 (och 2035) sedan utvecklingstakt från Scenario Transporteffektivt 20190529</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="5" shapeId="0" xr:uid="{43A05D46-7D5C-4E3A-9111-C2E49E53B8F2}">
+    <comment ref="A16" authorId="5" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Bensin=Otto</t>
+        </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="6" shapeId="0" xr:uid="{88AB02D8-4CA1-4C85-B8A3-8EAC71FECC61}">
+    <comment ref="F16" authorId="6" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Bensin=Otto</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -176,7 +270,7 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={B4B6D497-5A1B-4603-A45E-91F207B6C717}</author>
     <author>tc={AC072F96-4044-4E41-8BF2-F78319CB6BD0}</author>
@@ -216,295 +310,619 @@
     <author>tc={764C37F7-8F81-41BC-8B14-3B15CBD6537D}</author>
   </authors>
   <commentList>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{B4B6D497-5A1B-4603-A45E-91F207B6C717}">
+    <comment ref="D11" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Lindblom Helen, PLkvm:
 År 2019 gjordes ingen indexuppräkning med +2 %. Förslaget var dock att återinföra uppräkningen 2020. I efterhand blev det inte +2% 2020 heller, men i denna version av scenarioverktyget behåller vi antagandet som vi haft i scenarioarbetet under 2019. </t>
+        </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="1" shapeId="0" xr:uid="{AC072F96-4044-4E41-8BF2-F78319CB6BD0}">
+    <comment ref="E12" authorId="1" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="2" shapeId="0" xr:uid="{5C1BB38A-E2F8-45BC-9116-D53A5EF1DEB5}">
+    <comment ref="G12" authorId="2" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="3" shapeId="0" xr:uid="{F69EFCD4-6E93-4840-9CC7-CA40AB8C4435}">
+    <comment ref="I12" authorId="3" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="4" shapeId="0" xr:uid="{5A328B18-32CB-4BC1-8C93-D0EFBDA9001D}">
+    <comment ref="E14" authorId="4" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="5" shapeId="0" xr:uid="{AC08826A-35E8-41BB-ACE1-5811ACC708B9}">
+    <comment ref="G14" authorId="5" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I14" authorId="6" shapeId="0" xr:uid="{B1932D88-E2BA-4932-9C47-4DD1075204EC}">
+    <comment ref="I14" authorId="6" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E15" authorId="7" shapeId="0" xr:uid="{E06F340C-C181-427B-8DFA-22C5672FC231}">
+    <comment ref="E15" authorId="7" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G15" authorId="8" shapeId="0" xr:uid="{37C21FFB-FADA-4469-9D15-68303D0259E8}">
+    <comment ref="G15" authorId="8" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="9" shapeId="0" xr:uid="{9F7AF269-B33C-4C93-98F2-7436DFAD16D9}">
+    <comment ref="I15" authorId="9" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="10" shapeId="0" xr:uid="{2A5F67EA-2F3E-4E9F-87BC-C0D52EA57B1F}">
+    <comment ref="D30" authorId="10" shapeId="0">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Lindblom Helen, PLkvm:
 År 2019 gjordes ingen indexuppräkning med +2 %. Förslaget var dock att återinföra uppräkningen 2020. I efterhand blev det inte +2% 2020 heller, men i denna version av scenarioverktyget behåller vi antagandet som vi haft i scenarioarbetet under 2019. </t>
+        </r>
       </text>
     </comment>
-    <comment ref="E31" authorId="11" shapeId="0" xr:uid="{92F59C0E-ED7F-4E18-AEB2-C6334122588F}">
+    <comment ref="E31" authorId="11" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G31" authorId="12" shapeId="0" xr:uid="{0B408D22-4796-4F56-A8B9-BC08D535EA2E}">
+    <comment ref="G31" authorId="12" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I31" authorId="13" shapeId="0" xr:uid="{FE52B91A-A25B-4DC5-9F41-FB4C404182C2}">
+    <comment ref="I31" authorId="13" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E33" authorId="14" shapeId="0" xr:uid="{1E890709-6708-4E16-A7AE-4687A31990C2}">
+    <comment ref="E33" authorId="14" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G33" authorId="15" shapeId="0" xr:uid="{49B47804-5B36-445B-B25C-96B3D839C9A4}">
+    <comment ref="G33" authorId="15" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="16" shapeId="0" xr:uid="{5968B889-19FB-4CED-B335-46BF09CB4C0C}">
+    <comment ref="I33" authorId="16" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E34" authorId="17" shapeId="0" xr:uid="{AED4F88E-0CE8-4197-B5D6-141C1A9793DE}">
+    <comment ref="E34" authorId="17" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G34" authorId="18" shapeId="0" xr:uid="{7CD5509F-5D51-45EF-A943-13A86128F292}">
+    <comment ref="G34" authorId="18" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I34" authorId="19" shapeId="0" xr:uid="{72D31CE4-43EA-42B2-88F5-6284A31D9398}">
+    <comment ref="I34" authorId="19" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D49" authorId="20" shapeId="0" xr:uid="{4CCEA439-7CC9-4316-BBC8-6E59DE461C72}">
+    <comment ref="D49" authorId="20" shapeId="0">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Lindblom Helen, PLkvm:
 År 2019 gjordes ingen indexuppräkning med +2 %. Förslaget var dock att återinföra uppräkningen 2020. I efterhand blev det inte +2% 2020 heller, men i denna version av scenarioverktyget behåller vi antagandet som vi haft i scenarioarbetet under 2019. </t>
+        </r>
       </text>
     </comment>
-    <comment ref="E50" authorId="21" shapeId="0" xr:uid="{2BBC4C0F-2BDC-4463-94F0-A82DEA1DD17A}">
+    <comment ref="E50" authorId="21" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G50" authorId="22" shapeId="0" xr:uid="{B889FB77-4627-425B-B3B7-4141371CE06A}">
+    <comment ref="G50" authorId="22" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I50" authorId="23" shapeId="0" xr:uid="{D4EF19B2-D714-4D82-ABC1-68AB699437A0}">
+    <comment ref="I50" authorId="23" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E52" authorId="24" shapeId="0" xr:uid="{1711952F-029F-4138-94C3-B5D6E16E9E7D}">
+    <comment ref="E52" authorId="24" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G52" authorId="25" shapeId="0" xr:uid="{44E046A7-CD10-4068-B4D8-07A5D9AE4576}">
+    <comment ref="G52" authorId="25" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I52" authorId="26" shapeId="0" xr:uid="{8BFAF0CB-59B0-4D5E-B922-F078CFD47CF8}">
+    <comment ref="I52" authorId="26" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E53" authorId="27" shapeId="0" xr:uid="{25362C46-7BFC-42F4-8F6C-FA3B5097A282}">
+    <comment ref="E53" authorId="27" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G53" authorId="28" shapeId="0" xr:uid="{D7B56144-FC8E-400E-A05A-0B6479E630EC}">
+    <comment ref="G53" authorId="28" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I53" authorId="29" shapeId="0" xr:uid="{22CE925C-3AD8-4AB9-A6C2-7F053A70B6DB}">
+    <comment ref="I53" authorId="29" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E66" authorId="30" shapeId="0" xr:uid="{5CE36426-2062-4091-9F82-CDE40234B35A}">
+    <comment ref="E66" authorId="30" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G66" authorId="31" shapeId="0" xr:uid="{40742653-2E1C-479A-ACE6-ADBEE9A07022}">
+    <comment ref="G66" authorId="31" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I66" authorId="32" shapeId="0" xr:uid="{4FC6A6C5-694F-490F-AB13-616A2B1B4C38}">
+    <comment ref="I66" authorId="32" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E79" authorId="33" shapeId="0" xr:uid="{E5E5122E-32ED-4E45-A0B7-EA5E8C906BDC}">
+    <comment ref="E79" authorId="33" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G79" authorId="34" shapeId="0" xr:uid="{A8EDEC94-12CF-4D05-87EB-F0C16EBD5C39}">
+    <comment ref="G79" authorId="34" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I79" authorId="35" shapeId="0" xr:uid="{764C37F7-8F81-41BC-8B14-3B15CBD6537D}">
+    <comment ref="I79" authorId="35" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Linjär utveckling antas mellan 2017 och 2040.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -512,17 +930,26 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={08B1590D-88F0-46FB-A528-251160639D83}</author>
   </authors>
   <commentList>
-    <comment ref="V9" authorId="0" shapeId="0" xr:uid="{08B1590D-88F0-46FB-A528-251160639D83}">
+    <comment ref="V9" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ev. liten justering beroende på vilken drivmedelsfördelning som använts i förebearbetning</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -2346,7 +2773,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
@@ -2356,7 +2783,7 @@
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
     <numFmt numFmtId="169" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2645,12 +3072,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -6057,35 +6478,35 @@
     </xf>
   </cellXfs>
   <cellStyles count="29">
-    <cellStyle name="Beräkning 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Beräkning 2" xfId="13"/>
     <cellStyle name="Calculation" xfId="7" builtinId="22"/>
     <cellStyle name="Comma" xfId="28" builtinId="3"/>
-    <cellStyle name="Förklarande text 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Förklarande text 2" xfId="14"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8"/>
-    <cellStyle name="Indata 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Indata 2" xfId="12"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
-    <cellStyle name="Länkat rubrikår" xfId="10" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Neutral 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Länkat rubrikår" xfId="10"/>
+    <cellStyle name="Neutral 2" xfId="11"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 12" xfId="19" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 2 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 2 4" xfId="22" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Normal 3" xfId="17" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Normal 4" xfId="6" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Normal 4 2" xfId="20" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Normal 5" xfId="23" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Normal 6" xfId="21" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Normal 7" xfId="24" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Normal 8 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Normal 9" xfId="4" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 12" xfId="19"/>
+    <cellStyle name="Normal 2" xfId="9"/>
+    <cellStyle name="Normal 2 2" xfId="16"/>
+    <cellStyle name="Normal 2 4" xfId="22"/>
+    <cellStyle name="Normal 3" xfId="17"/>
+    <cellStyle name="Normal 4" xfId="6"/>
+    <cellStyle name="Normal 4 2" xfId="20"/>
+    <cellStyle name="Normal 5" xfId="23"/>
+    <cellStyle name="Normal 6" xfId="21"/>
+    <cellStyle name="Normal 7" xfId="24"/>
+    <cellStyle name="Normal 8 2" xfId="3"/>
+    <cellStyle name="Normal 9" xfId="4"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Procent 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Procent 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Procent 4" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Procent 6" xfId="18" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Rubrik 2 PS" xfId="8" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Tusental 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Procent 2" xfId="15"/>
+    <cellStyle name="Procent 3" xfId="5"/>
+    <cellStyle name="Procent 4" xfId="25"/>
+    <cellStyle name="Procent 6" xfId="18"/>
+    <cellStyle name="Rubrik 2 PS" xfId="8"/>
+    <cellStyle name="Tusental 2" xfId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -10415,7 +10836,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Ändringar"/>
@@ -10481,7 +10902,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Framsida "/>
@@ -11158,13 +11579,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFD70000"/>
   </sheetPr>
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -11428,9 +11849,9 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{D5689ABB-F1F5-4B9E-BD19-C42DA9EE24B5}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{8EB9627A-A718-4904-B623-61B02839A574}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -11438,7 +11859,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -17786,7 +18207,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -27981,7 +28402,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -31094,13 +31515,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Indata - Fordon och Trafik'!$K$5:$K$6</xm:f>
           </x14:formula1>
           <xm:sqref>D17:G17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Indata - Fordon och Trafik'!$K$9:$K$11</xm:f>
           </x14:formula1>
@@ -31113,7 +31534,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -33796,7 +34217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -33829,16 +34250,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:D272"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
-      <selection pane="topRight" activeCell="C72" sqref="C72"/>
+      <selection pane="topRight" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35869,7 +36290,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFD2D2D2"/>
   </sheetPr>
@@ -36699,7 +37120,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFD2D2D2"/>
   </sheetPr>
@@ -37977,7 +38398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFD2D2D2"/>
   </sheetPr>
@@ -38725,7 +39146,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>

</xml_diff>